<commit_message>
Finis le projet time series en une journée
</commit_message>
<xml_diff>
--- a/data/All_Datasets.xlsx
+++ b/data/All_Datasets.xlsx
@@ -4794,7 +4794,7 @@
         <v>414</v>
       </c>
       <c r="E118" t="n">
-        <v>889</v>
+        <v>849</v>
       </c>
     </row>
     <row r="119">
@@ -5083,7 +5083,7 @@
         <v>469</v>
       </c>
       <c r="E135" t="n">
-        <v>1089</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="136">
@@ -5270,7 +5270,7 @@
         <v>501</v>
       </c>
       <c r="E146" t="n">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="147">

</xml_diff>